<commit_message>
Added wireframe for country profile and sample traffic light
</commit_message>
<xml_diff>
--- a/oscar/GDP_data 2017-2020.xlsx
+++ b/oscar/GDP_data 2017-2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Abyss Web Server\Cirrodocs\gqueers_space_apps\oscar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenmarylabao-barrameda/Websites/gqueers_space_apps/oscar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FE2BCA-4CD1-44BC-93F5-B3976C783590}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C964F2-E9A9-B848-BE1E-E8A86A831372}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="150" windowWidth="15750" windowHeight="9855" xr2:uid="{C8641F41-FA25-4BC3-9299-9AF5B9B1BC70}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C8641F41-FA25-4BC3-9299-9AF5B9B1BC70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>Q1</t>
   </si>
@@ -69,6 +67,87 @@
   </si>
   <si>
     <t>Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legend: </t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>0-2.5</t>
+  </si>
+  <si>
+    <t>2.5-5</t>
+  </si>
+  <si>
+    <t>&gt;5</t>
+  </si>
+  <si>
+    <t>Manageable</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Night Light </t>
+  </si>
+  <si>
+    <t>NO2</t>
+  </si>
+  <si>
+    <t>Mobility Score</t>
+  </si>
+  <si>
+    <t>Covid-19 Growth</t>
+  </si>
+  <si>
+    <t>Economy of Japan is resilient</t>
+  </si>
+  <si>
+    <t>COUNTRY INSIGHTS: PHILIPPINES</t>
+  </si>
+  <si>
+    <t>COUNTRY INSIGHTS: JAPAN</t>
+  </si>
+  <si>
+    <t>Economy of Philippines need</t>
+  </si>
+  <si>
+    <t>immediate action</t>
+  </si>
+  <si>
+    <t>COUNTRY INSIGHTS: SINGAPORE</t>
+  </si>
+  <si>
+    <t>Economy of Singapore undergoing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderate change in GDP. </t>
+  </si>
+  <si>
+    <t>COUNTRY INSIGHTS :</t>
+  </si>
+  <si>
+    <t>screenshot Night Light</t>
+  </si>
+  <si>
+    <t>screenshot NO2</t>
+  </si>
+  <si>
+    <t>2020-2019</t>
+  </si>
+  <si>
+    <t>DeltaSample</t>
   </si>
 </sst>
 </file>
@@ -90,15 +169,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -106,13 +203,119 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,20 +630,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{325EF17B-8AB5-4964-A930-FFE80F375863}">
-  <dimension ref="B1:I17"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -466,7 +670,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>2017</v>
       </c>
@@ -492,7 +696,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -515,7 +719,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -538,7 +742,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -560,8 +764,18 @@
       <c r="I5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="4"/>
+    </row>
+    <row r="6" spans="2:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2018</v>
       </c>
@@ -586,8 +800,20 @@
       <c r="I6">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="11"/>
+      <c r="K6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="18"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -609,8 +835,20 @@
       <c r="I7">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="11"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="18"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -632,8 +870,24 @@
       <c r="I8">
         <v>-0.8</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="11"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="8"/>
+      <c r="S8" s="18"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -655,8 +909,18 @@
       <c r="I9">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="11"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="18"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>2019</v>
       </c>
@@ -681,8 +945,18 @@
       <c r="I10">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="11"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="18"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>1</v>
       </c>
@@ -704,8 +978,18 @@
       <c r="I11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="11"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="18"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>2</v>
       </c>
@@ -727,8 +1011,24 @@
       <c r="I12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="11"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="R12" s="8"/>
+      <c r="S12" s="18"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>2020</v>
       </c>
@@ -753,8 +1053,18 @@
       <c r="I13">
         <v>-1.9</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="11"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="18"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>0</v>
       </c>
@@ -773,24 +1083,479 @@
       <c r="I14">
         <v>-0.9</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="11"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="18"/>
+    </row>
+    <row r="15" spans="2:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="11"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="18"/>
+    </row>
+    <row r="16" spans="2:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="J16" s="11"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="18"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>3</v>
       </c>
+      <c r="J17" s="11"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="18"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <f>D14-D13</f>
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:I18" si="0">E14-E13</f>
+        <v>-0.4</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>-6.8999999999999995</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>-5.3</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="J18" s="11"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R18" s="8"/>
+      <c r="S18" s="18"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="11"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="18"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J20" s="11"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="18"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="11"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="18"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="R22" s="8"/>
+      <c r="S22" s="18"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="18"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="11"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="18"/>
+    </row>
+    <row r="25" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="11"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="18"/>
+    </row>
+    <row r="26" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="11"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="18"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J27" s="11"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="18"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J28" s="11"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28" s="6"/>
+      <c r="O28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R28" s="8"/>
+      <c r="S28" s="18"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J29" s="11"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="18"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J30" s="11"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="18"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J31" s="11"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="18"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J32" s="11"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="R32" s="8"/>
+      <c r="S32" s="18"/>
+    </row>
+    <row r="33" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J33" s="11"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="18"/>
+    </row>
+    <row r="34" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J34" s="11"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="18"/>
+    </row>
+    <row r="35" spans="10:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J35" s="11"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="18"/>
+    </row>
+    <row r="36" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J36" s="11"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="18"/>
+    </row>
+    <row r="37" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J37" s="11"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="18"/>
+    </row>
+    <row r="38" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J38" s="11"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="18"/>
+    </row>
+    <row r="39" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J39" s="11"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="18"/>
+    </row>
+    <row r="40" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J40" s="11"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="18"/>
+    </row>
+    <row r="41" spans="10:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J41" s="12"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="19"/>
     </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="O22:P25"/>
+    <mergeCell ref="Q22:R25"/>
+    <mergeCell ref="O28:P31"/>
+    <mergeCell ref="Q28:R31"/>
+    <mergeCell ref="O32:P35"/>
+    <mergeCell ref="Q32:R35"/>
+    <mergeCell ref="O8:P11"/>
+    <mergeCell ref="Q8:R11"/>
+    <mergeCell ref="O12:P15"/>
+    <mergeCell ref="Q12:R15"/>
+    <mergeCell ref="O18:P21"/>
+    <mergeCell ref="Q18:R21"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="D18:I18">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>